<commit_message>
Bug fix for defuse loading
</commit_message>
<xml_diff>
--- a/Base/TileMap/Formatting/Level4.xlsx
+++ b/Base/TileMap/Formatting/Level4.xlsx
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="Level4" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -164,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +363,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -523,11 +536,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -849,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE56"/>
+  <dimension ref="A1:BI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BJ23" sqref="BJ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,91 +1425,91 @@
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
-      <c r="AH4">
-        <v>0</v>
-      </c>
-      <c r="AI4">
-        <v>0</v>
-      </c>
-      <c r="AJ4">
-        <v>0</v>
-      </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
-      <c r="AM4">
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0</v>
+      </c>
+      <c r="T4" s="5">
+        <v>0</v>
+      </c>
+      <c r="U4" s="5">
+        <v>0</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5">
+        <v>0</v>
+      </c>
+      <c r="X4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="5">
         <v>0</v>
       </c>
       <c r="AN4">
@@ -1926,8 +1941,8 @@
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7">
-        <v>0</v>
+      <c r="J7" s="3">
+        <v>22</v>
       </c>
       <c r="K7" s="1">
         <v>1</v>
@@ -2410,7 +2425,7 @@
       <c r="BC9">
         <v>0</v>
       </c>
-      <c r="BD9">
+      <c r="BD9" s="5">
         <v>0</v>
       </c>
       <c r="BE9" s="1">
@@ -2442,11 +2457,11 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1">
-        <v>1</v>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
       </c>
       <c r="K10" s="1">
         <v>1</v>
@@ -2454,11 +2469,11 @@
       <c r="L10" s="1">
         <v>1</v>
       </c>
-      <c r="M10" s="1">
-        <v>1</v>
-      </c>
-      <c r="N10" s="1">
-        <v>1</v>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -2478,11 +2493,11 @@
       <c r="T10">
         <v>0</v>
       </c>
-      <c r="U10" s="1">
-        <v>1</v>
-      </c>
-      <c r="V10" s="1">
-        <v>1</v>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
       </c>
       <c r="W10" s="1">
         <v>1</v>
@@ -2490,11 +2505,11 @@
       <c r="X10" s="1">
         <v>1</v>
       </c>
-      <c r="Y10" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="1">
-        <v>1</v>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
       </c>
       <c r="AA10">
         <v>0</v>
@@ -2514,11 +2529,11 @@
       <c r="AF10">
         <v>0</v>
       </c>
-      <c r="AG10" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH10" s="1">
-        <v>1</v>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
       </c>
       <c r="AI10" s="1">
         <v>1</v>
@@ -2526,11 +2541,11 @@
       <c r="AJ10" s="1">
         <v>1</v>
       </c>
-      <c r="AK10" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL10" s="1">
-        <v>1</v>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
       </c>
       <c r="AM10">
         <v>0</v>
@@ -2583,7 +2598,7 @@
       <c r="BC10">
         <v>0</v>
       </c>
-      <c r="BD10">
+      <c r="BD10" s="5">
         <v>0</v>
       </c>
       <c r="BE10" s="1">
@@ -2615,11 +2630,11 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1">
-        <v>1</v>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
       </c>
       <c r="K11" s="1">
         <v>1</v>
@@ -2627,11 +2642,11 @@
       <c r="L11" s="1">
         <v>1</v>
       </c>
-      <c r="M11" s="1">
-        <v>1</v>
-      </c>
-      <c r="N11" s="1">
-        <v>1</v>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -2651,11 +2666,11 @@
       <c r="T11">
         <v>0</v>
       </c>
-      <c r="U11" s="1">
-        <v>1</v>
-      </c>
-      <c r="V11" s="1">
-        <v>1</v>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
       </c>
       <c r="W11" s="1">
         <v>1</v>
@@ -2663,11 +2678,11 @@
       <c r="X11" s="1">
         <v>1</v>
       </c>
-      <c r="Y11" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="1">
-        <v>1</v>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
       </c>
       <c r="AA11">
         <v>0</v>
@@ -2687,11 +2702,11 @@
       <c r="AF11">
         <v>0</v>
       </c>
-      <c r="AG11" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="1">
-        <v>1</v>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
       </c>
       <c r="AI11" s="1">
         <v>1</v>
@@ -2699,11 +2714,11 @@
       <c r="AJ11" s="1">
         <v>1</v>
       </c>
-      <c r="AK11" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL11" s="1">
-        <v>1</v>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
       </c>
       <c r="AM11">
         <v>0</v>
@@ -2756,7 +2771,7 @@
       <c r="BC11">
         <v>0</v>
       </c>
-      <c r="BD11">
+      <c r="BD11" s="5">
         <v>0</v>
       </c>
       <c r="BE11" s="1">
@@ -2767,20 +2782,20 @@
       <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12" s="3">
-        <v>22</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -2788,23 +2803,23 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -2812,11 +2827,11 @@
       <c r="P12">
         <v>0</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
+      <c r="Q12" s="1">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1">
+        <v>1</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -2824,23 +2839,23 @@
       <c r="T12">
         <v>0</v>
       </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
-      <c r="Z12">
-        <v>0</v>
+      <c r="U12" s="1">
+        <v>1</v>
+      </c>
+      <c r="V12" s="1">
+        <v>1</v>
+      </c>
+      <c r="W12" s="1">
+        <v>1</v>
+      </c>
+      <c r="X12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>1</v>
       </c>
       <c r="AA12">
         <v>0</v>
@@ -2848,11 +2863,11 @@
       <c r="AB12">
         <v>0</v>
       </c>
-      <c r="AC12">
-        <v>0</v>
-      </c>
-      <c r="AD12">
-        <v>0</v>
+      <c r="AC12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>1</v>
       </c>
       <c r="AE12">
         <v>0</v>
@@ -2860,23 +2875,23 @@
       <c r="AF12">
         <v>0</v>
       </c>
-      <c r="AG12">
-        <v>0</v>
-      </c>
-      <c r="AH12">
-        <v>0</v>
-      </c>
-      <c r="AI12">
-        <v>0</v>
-      </c>
-      <c r="AJ12">
-        <v>0</v>
-      </c>
-      <c r="AK12">
-        <v>0</v>
-      </c>
-      <c r="AL12">
-        <v>0</v>
+      <c r="AG12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>1</v>
       </c>
       <c r="AM12">
         <v>0</v>
@@ -2884,41 +2899,41 @@
       <c r="AN12">
         <v>0</v>
       </c>
-      <c r="AO12">
-        <v>0</v>
-      </c>
-      <c r="AP12">
-        <v>0</v>
-      </c>
-      <c r="AQ12">
-        <v>0</v>
-      </c>
-      <c r="AR12">
-        <v>0</v>
-      </c>
-      <c r="AS12">
-        <v>0</v>
-      </c>
-      <c r="AT12">
-        <v>0</v>
-      </c>
-      <c r="AU12">
-        <v>0</v>
-      </c>
-      <c r="AV12">
-        <v>0</v>
-      </c>
-      <c r="AW12">
-        <v>0</v>
-      </c>
-      <c r="AX12">
-        <v>0</v>
-      </c>
-      <c r="AY12">
-        <v>0</v>
-      </c>
-      <c r="AZ12" s="3">
-        <v>22</v>
+      <c r="AO12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ12" s="1">
+        <v>1</v>
       </c>
       <c r="BA12" s="1">
         <v>1</v>
@@ -2929,7 +2944,7 @@
       <c r="BC12">
         <v>0</v>
       </c>
-      <c r="BD12">
+      <c r="BD12" s="5">
         <v>0</v>
       </c>
       <c r="BE12" s="1">
@@ -2940,20 +2955,20 @@
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -2961,23 +2976,23 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -2985,11 +3000,11 @@
       <c r="P13">
         <v>0</v>
       </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
+      <c r="Q13" s="1">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1">
+        <v>1</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -2997,23 +3012,23 @@
       <c r="T13">
         <v>0</v>
       </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="Z13">
-        <v>0</v>
+      <c r="U13" s="1">
+        <v>1</v>
+      </c>
+      <c r="V13" s="1">
+        <v>1</v>
+      </c>
+      <c r="W13" s="1">
+        <v>1</v>
+      </c>
+      <c r="X13" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>1</v>
       </c>
       <c r="AA13">
         <v>0</v>
@@ -3021,11 +3036,11 @@
       <c r="AB13">
         <v>0</v>
       </c>
-      <c r="AC13">
-        <v>0</v>
-      </c>
-      <c r="AD13">
-        <v>0</v>
+      <c r="AC13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>1</v>
       </c>
       <c r="AE13">
         <v>0</v>
@@ -3033,23 +3048,23 @@
       <c r="AF13">
         <v>0</v>
       </c>
-      <c r="AG13">
-        <v>0</v>
-      </c>
-      <c r="AH13">
-        <v>0</v>
-      </c>
-      <c r="AI13">
-        <v>0</v>
-      </c>
-      <c r="AJ13">
-        <v>0</v>
-      </c>
-      <c r="AK13">
-        <v>0</v>
-      </c>
-      <c r="AL13">
-        <v>0</v>
+      <c r="AG13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="1">
+        <v>1</v>
       </c>
       <c r="AM13">
         <v>0</v>
@@ -3057,41 +3072,41 @@
       <c r="AN13">
         <v>0</v>
       </c>
-      <c r="AO13">
-        <v>0</v>
-      </c>
-      <c r="AP13">
-        <v>0</v>
-      </c>
-      <c r="AQ13">
-        <v>0</v>
-      </c>
-      <c r="AR13">
-        <v>0</v>
-      </c>
-      <c r="AS13">
-        <v>0</v>
-      </c>
-      <c r="AT13">
-        <v>0</v>
-      </c>
-      <c r="AU13">
-        <v>0</v>
-      </c>
-      <c r="AV13">
-        <v>0</v>
-      </c>
-      <c r="AW13">
-        <v>0</v>
-      </c>
-      <c r="AX13">
-        <v>0</v>
-      </c>
-      <c r="AY13">
-        <v>0</v>
-      </c>
-      <c r="AZ13">
-        <v>0</v>
+      <c r="AO13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ13" s="1">
+        <v>1</v>
       </c>
       <c r="BA13" s="1">
         <v>1</v>
@@ -3102,7 +3117,7 @@
       <c r="BC13">
         <v>0</v>
       </c>
-      <c r="BD13">
+      <c r="BD13" s="5">
         <v>0</v>
       </c>
       <c r="BE13" s="1">
@@ -3113,8 +3128,8 @@
       <c r="A14" s="1">
         <v>1</v>
       </c>
-      <c r="B14">
-        <v>0</v>
+      <c r="B14" s="3">
+        <v>22</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -3125,40 +3140,40 @@
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0</v>
+      </c>
+      <c r="O14" s="5">
+        <v>0</v>
+      </c>
+      <c r="P14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="5">
         <v>0</v>
       </c>
       <c r="R14">
@@ -3173,46 +3188,46 @@
       <c r="U14">
         <v>0</v>
       </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <v>0</v>
-      </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
-      <c r="AB14">
-        <v>0</v>
-      </c>
-      <c r="AC14">
-        <v>0</v>
-      </c>
-      <c r="AD14">
-        <v>0</v>
-      </c>
-      <c r="AE14">
-        <v>0</v>
-      </c>
-      <c r="AF14">
-        <v>0</v>
-      </c>
-      <c r="AG14">
-        <v>0</v>
-      </c>
-      <c r="AH14">
-        <v>0</v>
-      </c>
-      <c r="AI14">
+      <c r="V14" s="5">
+        <v>0</v>
+      </c>
+      <c r="W14" s="5">
+        <v>0</v>
+      </c>
+      <c r="X14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="5">
         <v>0</v>
       </c>
       <c r="AJ14">
@@ -3227,34 +3242,34 @@
       <c r="AM14">
         <v>0</v>
       </c>
-      <c r="AN14">
-        <v>0</v>
-      </c>
-      <c r="AO14">
-        <v>0</v>
-      </c>
-      <c r="AP14">
-        <v>0</v>
-      </c>
-      <c r="AQ14">
-        <v>0</v>
-      </c>
-      <c r="AR14">
-        <v>0</v>
-      </c>
-      <c r="AS14">
-        <v>0</v>
-      </c>
-      <c r="AT14">
-        <v>0</v>
-      </c>
-      <c r="AU14">
-        <v>0</v>
-      </c>
-      <c r="AV14">
-        <v>0</v>
-      </c>
-      <c r="AW14">
+      <c r="AN14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW14" s="5">
         <v>0</v>
       </c>
       <c r="AX14">
@@ -3263,8 +3278,8 @@
       <c r="AY14">
         <v>0</v>
       </c>
-      <c r="AZ14">
-        <v>0</v>
+      <c r="AZ14" s="3">
+        <v>22</v>
       </c>
       <c r="BA14" s="1">
         <v>1</v>
@@ -3275,7 +3290,7 @@
       <c r="BC14">
         <v>0</v>
       </c>
-      <c r="BD14">
+      <c r="BD14" s="5">
         <v>0</v>
       </c>
       <c r="BE14" s="1">
@@ -3448,7 +3463,7 @@
       <c r="BC15">
         <v>0</v>
       </c>
-      <c r="BD15">
+      <c r="BD15" s="5">
         <v>0</v>
       </c>
       <c r="BE15" s="1">
@@ -3606,7 +3621,7 @@
       <c r="AX16">
         <v>0</v>
       </c>
-      <c r="AY16">
+      <c r="AY16" s="5">
         <v>0</v>
       </c>
       <c r="AZ16">
@@ -3621,14 +3636,14 @@
       <c r="BC16">
         <v>0</v>
       </c>
-      <c r="BD16">
+      <c r="BD16" s="5">
         <v>0</v>
       </c>
       <c r="BE16" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -3779,7 +3794,7 @@
       <c r="AX17">
         <v>0</v>
       </c>
-      <c r="AY17">
+      <c r="AY17" s="5">
         <v>0</v>
       </c>
       <c r="AZ17">
@@ -3794,34 +3809,34 @@
       <c r="BC17">
         <v>0</v>
       </c>
-      <c r="BD17">
+      <c r="BD17" s="5">
         <v>0</v>
       </c>
       <c r="BE17" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
       <c r="B18">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1">
         <v>1</v>
@@ -3952,7 +3967,7 @@
       <c r="AX18">
         <v>0</v>
       </c>
-      <c r="AY18">
+      <c r="AY18" s="5">
         <v>0</v>
       </c>
       <c r="AZ18">
@@ -3967,34 +3982,34 @@
       <c r="BC18">
         <v>0</v>
       </c>
-      <c r="BD18">
+      <c r="BD18" s="5">
         <v>0</v>
       </c>
       <c r="BE18" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
       <c r="B19">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
@@ -4125,7 +4140,7 @@
       <c r="AX19">
         <v>0</v>
       </c>
-      <c r="AY19">
+      <c r="AY19" s="5">
         <v>0</v>
       </c>
       <c r="AZ19">
@@ -4140,46 +4155,46 @@
       <c r="BC19">
         <v>0</v>
       </c>
-      <c r="BD19">
+      <c r="BD19" s="5">
         <v>0</v>
       </c>
       <c r="BE19" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1</v>
       </c>
       <c r="B20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K20">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>1</v>
@@ -4298,7 +4313,7 @@
       <c r="AX20">
         <v>0</v>
       </c>
-      <c r="AY20">
+      <c r="AY20" s="5">
         <v>0</v>
       </c>
       <c r="AZ20">
@@ -4313,46 +4328,46 @@
       <c r="BC20">
         <v>0</v>
       </c>
-      <c r="BD20">
+      <c r="BD20" s="5">
         <v>0</v>
       </c>
       <c r="BE20" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
       <c r="B21">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>25</v>
-      </c>
-      <c r="J21">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>0</v>
       </c>
       <c r="K21">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="L21" s="1">
         <v>1</v>
@@ -4471,7 +4486,7 @@
       <c r="AX21">
         <v>0</v>
       </c>
-      <c r="AY21">
+      <c r="AY21" s="5">
         <v>0</v>
       </c>
       <c r="AZ21">
@@ -4486,22 +4501,22 @@
       <c r="BC21">
         <v>0</v>
       </c>
-      <c r="BD21">
+      <c r="BD21" s="5">
         <v>0</v>
       </c>
       <c r="BE21" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1</v>
       </c>
       <c r="B22">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -4521,7 +4536,7 @@
       <c r="I22">
         <v>0</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="5">
         <v>0</v>
       </c>
       <c r="K22">
@@ -4644,7 +4659,7 @@
       <c r="AX22">
         <v>0</v>
       </c>
-      <c r="AY22">
+      <c r="AY22" s="5">
         <v>0</v>
       </c>
       <c r="AZ22">
@@ -4665,16 +4680,20 @@
       <c r="BE22" s="1">
         <v>1</v>
       </c>
+      <c r="BI22">
+        <f>51-4</f>
+        <v>47</v>
+      </c>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
       <c r="B23">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -4694,7 +4713,7 @@
       <c r="I23">
         <v>0</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="5">
         <v>0</v>
       </c>
       <c r="K23">
@@ -4730,8 +4749,8 @@
       <c r="U23">
         <v>0</v>
       </c>
-      <c r="V23">
-        <v>0</v>
+      <c r="V23" s="3">
+        <v>22</v>
       </c>
       <c r="W23" s="1">
         <v>1</v>
@@ -4739,8 +4758,8 @@
       <c r="X23" s="1">
         <v>1</v>
       </c>
-      <c r="Y23">
-        <v>0</v>
+      <c r="Y23" s="3">
+        <v>22</v>
       </c>
       <c r="Z23">
         <v>0</v>
@@ -4766,8 +4785,8 @@
       <c r="AG23">
         <v>0</v>
       </c>
-      <c r="AH23">
-        <v>0</v>
+      <c r="AH23" s="3">
+        <v>22</v>
       </c>
       <c r="AI23" s="1">
         <v>1</v>
@@ -4775,8 +4794,8 @@
       <c r="AJ23" s="1">
         <v>1</v>
       </c>
-      <c r="AK23">
-        <v>0</v>
+      <c r="AK23" s="3">
+        <v>22</v>
       </c>
       <c r="AL23">
         <v>0</v>
@@ -4802,8 +4821,8 @@
       <c r="AS23">
         <v>0</v>
       </c>
-      <c r="AT23">
-        <v>0</v>
+      <c r="AT23" s="3">
+        <v>22</v>
       </c>
       <c r="AU23" s="1">
         <v>1</v>
@@ -4817,7 +4836,7 @@
       <c r="AX23">
         <v>0</v>
       </c>
-      <c r="AY23">
+      <c r="AY23" s="5">
         <v>0</v>
       </c>
       <c r="AZ23">
@@ -4839,15 +4858,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1</v>
       </c>
       <c r="B24">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -4867,19 +4886,19 @@
       <c r="I24">
         <v>0</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
+      <c r="J24" s="5">
+        <v>0</v>
+      </c>
+      <c r="K24" s="5">
+        <v>0</v>
+      </c>
+      <c r="L24" s="5">
+        <v>0</v>
+      </c>
+      <c r="M24" s="5">
+        <v>0</v>
+      </c>
+      <c r="N24" s="5">
         <v>0</v>
       </c>
       <c r="O24">
@@ -4990,7 +5009,7 @@
       <c r="AX24">
         <v>0</v>
       </c>
-      <c r="AY24">
+      <c r="AY24" s="5">
         <v>0</v>
       </c>
       <c r="AZ24">
@@ -5012,20 +5031,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
       <c r="B25">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="5">
         <v>0</v>
       </c>
       <c r="F25">
@@ -5058,8 +5077,8 @@
       <c r="O25">
         <v>0</v>
       </c>
-      <c r="P25">
-        <v>0</v>
+      <c r="P25" s="3">
+        <v>22</v>
       </c>
       <c r="Q25" s="1">
         <v>1</v>
@@ -5157,8 +5176,8 @@
       <c r="AV25" s="1">
         <v>1</v>
       </c>
-      <c r="AW25">
-        <v>0</v>
+      <c r="AW25" s="3">
+        <v>22</v>
       </c>
       <c r="AX25">
         <v>0</v>
@@ -5185,366 +5204,366 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1</v>
       </c>
       <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1">
+        <v>1</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26" s="3">
+        <v>22</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AG26" s="3">
+        <v>22</v>
+      </c>
+      <c r="AH26">
+        <v>0</v>
+      </c>
+      <c r="AI26">
+        <v>0</v>
+      </c>
+      <c r="AJ26">
+        <v>0</v>
+      </c>
+      <c r="AK26">
+        <v>0</v>
+      </c>
+      <c r="AL26">
+        <v>0</v>
+      </c>
+      <c r="AM26">
+        <v>0</v>
+      </c>
+      <c r="AN26">
+        <v>0</v>
+      </c>
+      <c r="AO26" s="3">
+        <v>22</v>
+      </c>
+      <c r="AP26">
+        <v>0</v>
+      </c>
+      <c r="AQ26">
+        <v>0</v>
+      </c>
+      <c r="AR26">
+        <v>0</v>
+      </c>
+      <c r="AS26">
+        <v>0</v>
+      </c>
+      <c r="AT26">
+        <v>0</v>
+      </c>
+      <c r="AU26">
+        <v>0</v>
+      </c>
+      <c r="AV26">
+        <v>0</v>
+      </c>
+      <c r="AW26">
+        <v>0</v>
+      </c>
+      <c r="AX26">
+        <v>0</v>
+      </c>
+      <c r="AY26">
+        <v>0</v>
+      </c>
+      <c r="AZ26">
+        <v>0</v>
+      </c>
+      <c r="BA26">
+        <v>0</v>
+      </c>
+      <c r="BB26">
+        <v>0</v>
+      </c>
+      <c r="BC26">
+        <v>0</v>
+      </c>
+      <c r="BD26">
+        <v>0</v>
+      </c>
+      <c r="BE26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="M27" s="4">
         <v>25</v>
       </c>
-      <c r="C26">
-        <v>25</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1</v>
-      </c>
-      <c r="I26" s="1">
-        <v>1</v>
-      </c>
-      <c r="J26" s="1">
-        <v>1</v>
-      </c>
-      <c r="K26" s="1">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1">
-        <v>1</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <v>0</v>
-      </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-      <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="W26">
-        <v>0</v>
-      </c>
-      <c r="X26">
-        <v>0</v>
-      </c>
-      <c r="Y26">
-        <v>0</v>
-      </c>
-      <c r="Z26">
-        <v>0</v>
-      </c>
-      <c r="AA26">
-        <v>0</v>
-      </c>
-      <c r="AB26">
-        <v>0</v>
-      </c>
-      <c r="AC26">
-        <v>0</v>
-      </c>
-      <c r="AD26">
-        <v>0</v>
-      </c>
-      <c r="AE26">
-        <v>0</v>
-      </c>
-      <c r="AF26">
-        <v>0</v>
-      </c>
-      <c r="AG26">
-        <v>0</v>
-      </c>
-      <c r="AH26">
-        <v>0</v>
-      </c>
-      <c r="AI26">
-        <v>0</v>
-      </c>
-      <c r="AJ26">
-        <v>0</v>
-      </c>
-      <c r="AK26">
-        <v>0</v>
-      </c>
-      <c r="AL26">
-        <v>0</v>
-      </c>
-      <c r="AM26">
-        <v>0</v>
-      </c>
-      <c r="AN26">
-        <v>0</v>
-      </c>
-      <c r="AO26">
-        <v>0</v>
-      </c>
-      <c r="AP26">
-        <v>0</v>
-      </c>
-      <c r="AQ26">
-        <v>0</v>
-      </c>
-      <c r="AR26">
-        <v>0</v>
-      </c>
-      <c r="AS26">
-        <v>0</v>
-      </c>
-      <c r="AT26">
-        <v>0</v>
-      </c>
-      <c r="AU26">
-        <v>0</v>
-      </c>
-      <c r="AV26">
-        <v>0</v>
-      </c>
-      <c r="AW26">
-        <v>0</v>
-      </c>
-      <c r="AX26">
-        <v>0</v>
-      </c>
-      <c r="AY26">
-        <v>0</v>
-      </c>
-      <c r="AZ26">
-        <v>0</v>
-      </c>
-      <c r="BA26">
-        <v>0</v>
-      </c>
-      <c r="BB26">
-        <v>0</v>
-      </c>
-      <c r="BC26">
-        <v>0</v>
-      </c>
-      <c r="BD26">
-        <v>0</v>
-      </c>
-      <c r="BE26" s="1">
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27" s="5">
+        <v>0</v>
+      </c>
+      <c r="X27" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
+      <c r="AM27">
+        <v>0</v>
+      </c>
+      <c r="AN27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX27">
+        <v>0</v>
+      </c>
+      <c r="AY27">
+        <v>0</v>
+      </c>
+      <c r="AZ27">
+        <v>0</v>
+      </c>
+      <c r="BA27">
+        <v>0</v>
+      </c>
+      <c r="BB27">
+        <v>0</v>
+      </c>
+      <c r="BC27">
+        <v>0</v>
+      </c>
+      <c r="BD27">
+        <v>0</v>
+      </c>
+      <c r="BE27" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>1</v>
-      </c>
-      <c r="B27">
-        <v>25</v>
-      </c>
-      <c r="C27">
-        <v>25</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1">
-        <v>1</v>
-      </c>
-      <c r="I27" s="1">
-        <v>1</v>
-      </c>
-      <c r="J27" s="1">
-        <v>1</v>
-      </c>
-      <c r="K27" s="1">
-        <v>1</v>
-      </c>
-      <c r="L27" s="1">
-        <v>1</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-      <c r="T27">
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <v>0</v>
-      </c>
-      <c r="V27">
-        <v>0</v>
-      </c>
-      <c r="W27">
-        <v>0</v>
-      </c>
-      <c r="X27">
-        <v>0</v>
-      </c>
-      <c r="Y27">
-        <v>0</v>
-      </c>
-      <c r="Z27">
-        <v>0</v>
-      </c>
-      <c r="AA27">
-        <v>0</v>
-      </c>
-      <c r="AB27">
-        <v>0</v>
-      </c>
-      <c r="AC27">
-        <v>0</v>
-      </c>
-      <c r="AD27">
-        <v>0</v>
-      </c>
-      <c r="AE27">
-        <v>0</v>
-      </c>
-      <c r="AF27">
-        <v>0</v>
-      </c>
-      <c r="AG27">
-        <v>0</v>
-      </c>
-      <c r="AH27">
-        <v>0</v>
-      </c>
-      <c r="AI27">
-        <v>0</v>
-      </c>
-      <c r="AJ27">
-        <v>0</v>
-      </c>
-      <c r="AK27">
-        <v>0</v>
-      </c>
-      <c r="AL27">
-        <v>0</v>
-      </c>
-      <c r="AM27">
-        <v>0</v>
-      </c>
-      <c r="AN27">
-        <v>0</v>
-      </c>
-      <c r="AO27">
-        <v>0</v>
-      </c>
-      <c r="AP27">
-        <v>0</v>
-      </c>
-      <c r="AQ27">
-        <v>0</v>
-      </c>
-      <c r="AR27">
-        <v>0</v>
-      </c>
-      <c r="AS27">
-        <v>0</v>
-      </c>
-      <c r="AT27">
-        <v>0</v>
-      </c>
-      <c r="AU27">
-        <v>0</v>
-      </c>
-      <c r="AV27">
-        <v>0</v>
-      </c>
-      <c r="AW27">
-        <v>0</v>
-      </c>
-      <c r="AX27">
-        <v>0</v>
-      </c>
-      <c r="AY27">
-        <v>0</v>
-      </c>
-      <c r="AZ27">
-        <v>0</v>
-      </c>
-      <c r="BA27">
-        <v>0</v>
-      </c>
-      <c r="BB27">
-        <v>0</v>
-      </c>
-      <c r="BC27">
-        <v>0</v>
-      </c>
-      <c r="BD27">
-        <v>0</v>
-      </c>
-      <c r="BE27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
       <c r="B28">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="5">
         <v>0</v>
       </c>
       <c r="F28">
@@ -5577,8 +5596,8 @@
       <c r="O28">
         <v>0</v>
       </c>
-      <c r="P28">
-        <v>0</v>
+      <c r="P28" s="3">
+        <v>22</v>
       </c>
       <c r="Q28" s="1">
         <v>1</v>
@@ -5676,8 +5695,8 @@
       <c r="AV28" s="1">
         <v>1</v>
       </c>
-      <c r="AW28">
-        <v>0</v>
+      <c r="AW28" s="3">
+        <v>22</v>
       </c>
       <c r="AX28">
         <v>0</v>
@@ -5704,15 +5723,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1</v>
       </c>
       <c r="B29">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -5732,19 +5751,19 @@
       <c r="I29">
         <v>0</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
+      <c r="J29" s="5">
+        <v>0</v>
+      </c>
+      <c r="K29" s="5">
+        <v>0</v>
+      </c>
+      <c r="L29" s="5">
+        <v>0</v>
+      </c>
+      <c r="M29" s="5">
+        <v>0</v>
+      </c>
+      <c r="N29" s="5">
         <v>0</v>
       </c>
       <c r="O29">
@@ -5877,15 +5896,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1</v>
       </c>
       <c r="B30">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -5905,7 +5924,7 @@
       <c r="I30">
         <v>0</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="5">
         <v>0</v>
       </c>
       <c r="K30">
@@ -5941,8 +5960,8 @@
       <c r="U30">
         <v>0</v>
       </c>
-      <c r="V30">
-        <v>0</v>
+      <c r="V30" s="3">
+        <v>22</v>
       </c>
       <c r="W30" s="1">
         <v>1</v>
@@ -5950,8 +5969,8 @@
       <c r="X30" s="1">
         <v>1</v>
       </c>
-      <c r="Y30">
-        <v>0</v>
+      <c r="Y30" s="3">
+        <v>22</v>
       </c>
       <c r="Z30">
         <v>0</v>
@@ -5977,8 +5996,8 @@
       <c r="AG30">
         <v>0</v>
       </c>
-      <c r="AH30">
-        <v>0</v>
+      <c r="AH30" s="3">
+        <v>22</v>
       </c>
       <c r="AI30" s="1">
         <v>1</v>
@@ -5986,8 +6005,8 @@
       <c r="AJ30" s="1">
         <v>1</v>
       </c>
-      <c r="AK30">
-        <v>0</v>
+      <c r="AK30" s="3">
+        <v>22</v>
       </c>
       <c r="AL30">
         <v>0</v>
@@ -6013,8 +6032,8 @@
       <c r="AS30">
         <v>0</v>
       </c>
-      <c r="AT30">
-        <v>0</v>
+      <c r="AT30" s="3">
+        <v>22</v>
       </c>
       <c r="AU30" s="1">
         <v>1</v>
@@ -6028,7 +6047,7 @@
       <c r="AX30">
         <v>0</v>
       </c>
-      <c r="AY30">
+      <c r="AY30" s="5">
         <v>0</v>
       </c>
       <c r="AZ30">
@@ -6050,15 +6069,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1</v>
       </c>
       <c r="B31">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -6078,7 +6097,7 @@
       <c r="I31">
         <v>0</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="5">
         <v>0</v>
       </c>
       <c r="K31">
@@ -6201,7 +6220,7 @@
       <c r="AX31">
         <v>0</v>
       </c>
-      <c r="AY31">
+      <c r="AY31" s="5">
         <v>0</v>
       </c>
       <c r="AZ31">
@@ -6223,39 +6242,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1</v>
       </c>
       <c r="B32">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C32">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I32">
-        <v>25</v>
-      </c>
-      <c r="J32">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="J32" s="5">
+        <v>0</v>
       </c>
       <c r="K32">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="L32" s="1">
         <v>1</v>
@@ -6374,7 +6393,7 @@
       <c r="AX32">
         <v>0</v>
       </c>
-      <c r="AY32">
+      <c r="AY32" s="5">
         <v>0</v>
       </c>
       <c r="AZ32">
@@ -6401,34 +6420,34 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="K33">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="L33" s="1">
         <v>1</v>
@@ -6547,7 +6566,7 @@
       <c r="AX33">
         <v>0</v>
       </c>
-      <c r="AY33">
+      <c r="AY33" s="5">
         <v>0</v>
       </c>
       <c r="AZ33">
@@ -6574,22 +6593,22 @@
         <v>1</v>
       </c>
       <c r="B34">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C34">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H34" s="1">
         <v>1</v>
@@ -6720,7 +6739,7 @@
       <c r="AX34">
         <v>0</v>
       </c>
-      <c r="AY34">
+      <c r="AY34" s="5">
         <v>0</v>
       </c>
       <c r="AZ34">
@@ -6747,22 +6766,22 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F35">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1">
         <v>1</v>
@@ -6893,7 +6912,7 @@
       <c r="AX35">
         <v>0</v>
       </c>
-      <c r="AY35">
+      <c r="AY35" s="5">
         <v>0</v>
       </c>
       <c r="AZ35">
@@ -6905,7 +6924,7 @@
       <c r="BB35" s="1">
         <v>1</v>
       </c>
-      <c r="BC35">
+      <c r="BC35" s="5">
         <v>0</v>
       </c>
       <c r="BD35">
@@ -7066,7 +7085,7 @@
       <c r="AX36">
         <v>0</v>
       </c>
-      <c r="AY36">
+      <c r="AY36" s="5">
         <v>0</v>
       </c>
       <c r="AZ36">
@@ -7078,7 +7097,7 @@
       <c r="BB36" s="1">
         <v>1</v>
       </c>
-      <c r="BC36">
+      <c r="BC36" s="5">
         <v>0</v>
       </c>
       <c r="BD36">
@@ -7251,7 +7270,7 @@
       <c r="BB37" s="1">
         <v>1</v>
       </c>
-      <c r="BC37">
+      <c r="BC37" s="5">
         <v>0</v>
       </c>
       <c r="BD37">
@@ -7424,7 +7443,7 @@
       <c r="BB38" s="1">
         <v>1</v>
       </c>
-      <c r="BC38">
+      <c r="BC38" s="5">
         <v>0</v>
       </c>
       <c r="BD38">
@@ -7438,8 +7457,8 @@
       <c r="A39" s="1">
         <v>1</v>
       </c>
-      <c r="B39">
-        <v>0</v>
+      <c r="B39" s="3">
+        <v>22</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -7450,43 +7469,43 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>0</v>
-      </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-      <c r="M39">
-        <v>0</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39">
-        <v>0</v>
-      </c>
-      <c r="Q39">
-        <v>0</v>
-      </c>
-      <c r="R39">
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0</v>
+      </c>
+      <c r="K39" s="5">
+        <v>0</v>
+      </c>
+      <c r="L39" s="5">
+        <v>0</v>
+      </c>
+      <c r="M39" s="5">
+        <v>0</v>
+      </c>
+      <c r="N39" s="5">
+        <v>0</v>
+      </c>
+      <c r="O39" s="5">
+        <v>0</v>
+      </c>
+      <c r="P39" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>0</v>
+      </c>
+      <c r="R39" s="5">
         <v>0</v>
       </c>
       <c r="S39">
@@ -7501,43 +7520,43 @@
       <c r="V39">
         <v>0</v>
       </c>
-      <c r="W39">
-        <v>0</v>
-      </c>
-      <c r="X39">
-        <v>0</v>
-      </c>
-      <c r="Y39">
-        <v>0</v>
-      </c>
-      <c r="Z39">
-        <v>0</v>
-      </c>
-      <c r="AA39">
-        <v>0</v>
-      </c>
-      <c r="AB39">
-        <v>0</v>
-      </c>
-      <c r="AC39">
-        <v>0</v>
-      </c>
-      <c r="AD39">
-        <v>0</v>
-      </c>
-      <c r="AE39">
-        <v>0</v>
-      </c>
-      <c r="AF39">
-        <v>0</v>
-      </c>
-      <c r="AG39">
-        <v>0</v>
-      </c>
-      <c r="AH39">
-        <v>0</v>
-      </c>
-      <c r="AI39">
+      <c r="W39" s="5">
+        <v>0</v>
+      </c>
+      <c r="X39" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI39" s="5">
         <v>0</v>
       </c>
       <c r="AJ39">
@@ -7552,34 +7571,34 @@
       <c r="AM39">
         <v>0</v>
       </c>
-      <c r="AN39">
-        <v>0</v>
-      </c>
-      <c r="AO39">
-        <v>0</v>
-      </c>
-      <c r="AP39">
-        <v>0</v>
-      </c>
-      <c r="AQ39">
-        <v>0</v>
-      </c>
-      <c r="AR39">
-        <v>0</v>
-      </c>
-      <c r="AS39">
-        <v>0</v>
-      </c>
-      <c r="AT39">
-        <v>0</v>
-      </c>
-      <c r="AU39">
-        <v>0</v>
-      </c>
-      <c r="AV39">
-        <v>0</v>
-      </c>
-      <c r="AW39">
+      <c r="AN39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AW39" s="5">
         <v>0</v>
       </c>
       <c r="AX39">
@@ -7588,8 +7607,8 @@
       <c r="AY39">
         <v>0</v>
       </c>
-      <c r="AZ39">
-        <v>0</v>
+      <c r="AZ39" s="3">
+        <v>22</v>
       </c>
       <c r="BA39" s="1">
         <v>1</v>
@@ -7597,7 +7616,7 @@
       <c r="BB39" s="1">
         <v>1</v>
       </c>
-      <c r="BC39">
+      <c r="BC39" s="5">
         <v>0</v>
       </c>
       <c r="BD39">
@@ -7611,20 +7630,20 @@
       <c r="A40" s="1">
         <v>1</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -7632,23 +7651,23 @@
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
+      <c r="I40" s="1">
+        <v>1</v>
+      </c>
+      <c r="J40" s="1">
+        <v>1</v>
+      </c>
+      <c r="K40" s="1">
+        <v>1</v>
+      </c>
+      <c r="L40" s="1">
+        <v>1</v>
+      </c>
+      <c r="M40" s="1">
+        <v>1</v>
+      </c>
+      <c r="N40" s="1">
+        <v>1</v>
       </c>
       <c r="O40">
         <v>0</v>
@@ -7656,11 +7675,11 @@
       <c r="P40">
         <v>0</v>
       </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="R40">
-        <v>0</v>
+      <c r="Q40" s="1">
+        <v>1</v>
+      </c>
+      <c r="R40" s="1">
+        <v>1</v>
       </c>
       <c r="S40">
         <v>0</v>
@@ -7668,23 +7687,23 @@
       <c r="T40">
         <v>0</v>
       </c>
-      <c r="U40">
-        <v>0</v>
-      </c>
-      <c r="V40">
-        <v>0</v>
-      </c>
-      <c r="W40">
-        <v>0</v>
-      </c>
-      <c r="X40">
-        <v>0</v>
-      </c>
-      <c r="Y40">
-        <v>0</v>
-      </c>
-      <c r="Z40">
-        <v>0</v>
+      <c r="U40" s="1">
+        <v>1</v>
+      </c>
+      <c r="V40" s="1">
+        <v>1</v>
+      </c>
+      <c r="W40" s="1">
+        <v>1</v>
+      </c>
+      <c r="X40" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="1">
+        <v>1</v>
       </c>
       <c r="AA40">
         <v>0</v>
@@ -7692,11 +7711,11 @@
       <c r="AB40">
         <v>0</v>
       </c>
-      <c r="AC40">
-        <v>0</v>
-      </c>
-      <c r="AD40">
-        <v>0</v>
+      <c r="AC40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD40" s="1">
+        <v>1</v>
       </c>
       <c r="AE40">
         <v>0</v>
@@ -7704,23 +7723,23 @@
       <c r="AF40">
         <v>0</v>
       </c>
-      <c r="AG40">
-        <v>0</v>
-      </c>
-      <c r="AH40">
-        <v>0</v>
-      </c>
-      <c r="AI40">
-        <v>0</v>
-      </c>
-      <c r="AJ40">
-        <v>0</v>
-      </c>
-      <c r="AK40">
-        <v>0</v>
-      </c>
-      <c r="AL40">
-        <v>0</v>
+      <c r="AG40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL40" s="1">
+        <v>1</v>
       </c>
       <c r="AM40">
         <v>0</v>
@@ -7728,41 +7747,41 @@
       <c r="AN40">
         <v>0</v>
       </c>
-      <c r="AO40">
-        <v>0</v>
-      </c>
-      <c r="AP40">
-        <v>0</v>
-      </c>
-      <c r="AQ40">
-        <v>0</v>
-      </c>
-      <c r="AR40">
-        <v>0</v>
-      </c>
-      <c r="AS40">
-        <v>0</v>
-      </c>
-      <c r="AT40">
-        <v>0</v>
-      </c>
-      <c r="AU40">
-        <v>0</v>
-      </c>
-      <c r="AV40">
-        <v>0</v>
-      </c>
-      <c r="AW40">
-        <v>0</v>
-      </c>
-      <c r="AX40">
-        <v>0</v>
-      </c>
-      <c r="AY40">
-        <v>0</v>
-      </c>
-      <c r="AZ40">
-        <v>0</v>
+      <c r="AO40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ40" s="1">
+        <v>1</v>
       </c>
       <c r="BA40" s="1">
         <v>1</v>
@@ -7770,7 +7789,7 @@
       <c r="BB40" s="1">
         <v>1</v>
       </c>
-      <c r="BC40">
+      <c r="BC40" s="5">
         <v>0</v>
       </c>
       <c r="BD40">
@@ -7784,20 +7803,20 @@
       <c r="A41" s="1">
         <v>1</v>
       </c>
-      <c r="B41" s="3">
-        <v>22</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -7805,23 +7824,23 @@
       <c r="H41">
         <v>0</v>
       </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
+      <c r="I41" s="1">
+        <v>1</v>
+      </c>
+      <c r="J41" s="1">
+        <v>1</v>
+      </c>
+      <c r="K41" s="1">
+        <v>1</v>
+      </c>
+      <c r="L41" s="1">
+        <v>1</v>
+      </c>
+      <c r="M41" s="1">
+        <v>1</v>
+      </c>
+      <c r="N41" s="1">
+        <v>1</v>
       </c>
       <c r="O41">
         <v>0</v>
@@ -7829,11 +7848,11 @@
       <c r="P41">
         <v>0</v>
       </c>
-      <c r="Q41">
-        <v>0</v>
-      </c>
-      <c r="R41">
-        <v>0</v>
+      <c r="Q41" s="1">
+        <v>1</v>
+      </c>
+      <c r="R41" s="1">
+        <v>1</v>
       </c>
       <c r="S41">
         <v>0</v>
@@ -7841,23 +7860,23 @@
       <c r="T41">
         <v>0</v>
       </c>
-      <c r="U41">
-        <v>0</v>
-      </c>
-      <c r="V41">
-        <v>0</v>
-      </c>
-      <c r="W41">
-        <v>0</v>
-      </c>
-      <c r="X41">
-        <v>0</v>
-      </c>
-      <c r="Y41">
-        <v>0</v>
-      </c>
-      <c r="Z41">
-        <v>0</v>
+      <c r="U41" s="1">
+        <v>1</v>
+      </c>
+      <c r="V41" s="1">
+        <v>1</v>
+      </c>
+      <c r="W41" s="1">
+        <v>1</v>
+      </c>
+      <c r="X41" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="1">
+        <v>1</v>
       </c>
       <c r="AA41">
         <v>0</v>
@@ -7865,11 +7884,11 @@
       <c r="AB41">
         <v>0</v>
       </c>
-      <c r="AC41">
-        <v>0</v>
-      </c>
-      <c r="AD41">
-        <v>0</v>
+      <c r="AC41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD41" s="1">
+        <v>1</v>
       </c>
       <c r="AE41">
         <v>0</v>
@@ -7877,23 +7896,23 @@
       <c r="AF41">
         <v>0</v>
       </c>
-      <c r="AG41">
-        <v>0</v>
-      </c>
-      <c r="AH41">
-        <v>0</v>
-      </c>
-      <c r="AI41">
-        <v>0</v>
-      </c>
-      <c r="AJ41">
-        <v>0</v>
-      </c>
-      <c r="AK41">
-        <v>0</v>
-      </c>
-      <c r="AL41">
-        <v>0</v>
+      <c r="AG41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL41" s="1">
+        <v>1</v>
       </c>
       <c r="AM41">
         <v>0</v>
@@ -7901,41 +7920,41 @@
       <c r="AN41">
         <v>0</v>
       </c>
-      <c r="AO41">
-        <v>0</v>
-      </c>
-      <c r="AP41">
-        <v>0</v>
-      </c>
-      <c r="AQ41">
-        <v>0</v>
-      </c>
-      <c r="AR41">
-        <v>0</v>
-      </c>
-      <c r="AS41">
-        <v>0</v>
-      </c>
-      <c r="AT41">
-        <v>0</v>
-      </c>
-      <c r="AU41">
-        <v>0</v>
-      </c>
-      <c r="AV41">
-        <v>0</v>
-      </c>
-      <c r="AW41">
-        <v>0</v>
-      </c>
-      <c r="AX41">
-        <v>0</v>
-      </c>
-      <c r="AY41">
-        <v>0</v>
-      </c>
-      <c r="AZ41" s="3">
-        <v>22</v>
+      <c r="AO41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ41" s="1">
+        <v>1</v>
       </c>
       <c r="BA41" s="1">
         <v>1</v>
@@ -7943,7 +7962,7 @@
       <c r="BB41" s="1">
         <v>1</v>
       </c>
-      <c r="BC41">
+      <c r="BC41" s="5">
         <v>0</v>
       </c>
       <c r="BD41">
@@ -7978,11 +7997,11 @@
       <c r="H42">
         <v>0</v>
       </c>
-      <c r="I42" s="1">
-        <v>1</v>
-      </c>
-      <c r="J42" s="1">
-        <v>1</v>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
       </c>
       <c r="K42" s="1">
         <v>1</v>
@@ -7990,11 +8009,11 @@
       <c r="L42" s="1">
         <v>1</v>
       </c>
-      <c r="M42" s="1">
-        <v>1</v>
-      </c>
-      <c r="N42" s="1">
-        <v>1</v>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
       </c>
       <c r="O42">
         <v>0</v>
@@ -8014,11 +8033,11 @@
       <c r="T42">
         <v>0</v>
       </c>
-      <c r="U42" s="1">
-        <v>1</v>
-      </c>
-      <c r="V42" s="1">
-        <v>1</v>
+      <c r="U42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
       </c>
       <c r="W42" s="1">
         <v>1</v>
@@ -8026,11 +8045,11 @@
       <c r="X42" s="1">
         <v>1</v>
       </c>
-      <c r="Y42" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z42" s="1">
-        <v>1</v>
+      <c r="Y42">
+        <v>0</v>
+      </c>
+      <c r="Z42">
+        <v>0</v>
       </c>
       <c r="AA42">
         <v>0</v>
@@ -8050,11 +8069,11 @@
       <c r="AF42">
         <v>0</v>
       </c>
-      <c r="AG42" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH42" s="1">
-        <v>1</v>
+      <c r="AG42">
+        <v>0</v>
+      </c>
+      <c r="AH42">
+        <v>0</v>
       </c>
       <c r="AI42" s="1">
         <v>1</v>
@@ -8062,11 +8081,11 @@
       <c r="AJ42" s="1">
         <v>1</v>
       </c>
-      <c r="AK42" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL42" s="1">
-        <v>1</v>
+      <c r="AK42">
+        <v>0</v>
+      </c>
+      <c r="AL42">
+        <v>0</v>
       </c>
       <c r="AM42">
         <v>0</v>
@@ -8116,7 +8135,7 @@
       <c r="BB42" s="1">
         <v>1</v>
       </c>
-      <c r="BC42">
+      <c r="BC42" s="5">
         <v>0</v>
       </c>
       <c r="BD42">
@@ -8151,11 +8170,11 @@
       <c r="H43">
         <v>0</v>
       </c>
-      <c r="I43" s="1">
-        <v>1</v>
-      </c>
-      <c r="J43" s="1">
-        <v>1</v>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
       </c>
       <c r="K43" s="1">
         <v>1</v>
@@ -8163,11 +8182,11 @@
       <c r="L43" s="1">
         <v>1</v>
       </c>
-      <c r="M43" s="1">
-        <v>1</v>
-      </c>
-      <c r="N43" s="1">
-        <v>1</v>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
       </c>
       <c r="O43">
         <v>0</v>
@@ -8187,11 +8206,11 @@
       <c r="T43">
         <v>0</v>
       </c>
-      <c r="U43" s="1">
-        <v>1</v>
-      </c>
-      <c r="V43" s="1">
-        <v>1</v>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <v>0</v>
       </c>
       <c r="W43" s="1">
         <v>1</v>
@@ -8199,11 +8218,11 @@
       <c r="X43" s="1">
         <v>1</v>
       </c>
-      <c r="Y43" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z43" s="1">
-        <v>1</v>
+      <c r="Y43">
+        <v>0</v>
+      </c>
+      <c r="Z43">
+        <v>0</v>
       </c>
       <c r="AA43">
         <v>0</v>
@@ -8223,11 +8242,11 @@
       <c r="AF43">
         <v>0</v>
       </c>
-      <c r="AG43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH43" s="1">
-        <v>1</v>
+      <c r="AG43">
+        <v>0</v>
+      </c>
+      <c r="AH43">
+        <v>0</v>
       </c>
       <c r="AI43" s="1">
         <v>1</v>
@@ -8235,11 +8254,11 @@
       <c r="AJ43" s="1">
         <v>1</v>
       </c>
-      <c r="AK43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AL43" s="1">
-        <v>1</v>
+      <c r="AK43">
+        <v>0</v>
+      </c>
+      <c r="AL43">
+        <v>0</v>
       </c>
       <c r="AM43">
         <v>0</v>
@@ -8289,7 +8308,7 @@
       <c r="BB43" s="1">
         <v>1</v>
       </c>
-      <c r="BC43">
+      <c r="BC43" s="5">
         <v>0</v>
       </c>
       <c r="BD43">
@@ -8462,7 +8481,7 @@
       <c r="BB44" s="1">
         <v>1</v>
       </c>
-      <c r="BC44">
+      <c r="BC44" s="5">
         <v>0</v>
       </c>
       <c r="BD44">
@@ -8635,7 +8654,7 @@
       <c r="BB45" s="1">
         <v>1</v>
       </c>
-      <c r="BC45">
+      <c r="BC45" s="5">
         <v>0</v>
       </c>
       <c r="BD45">
@@ -8673,8 +8692,8 @@
       <c r="I46">
         <v>0</v>
       </c>
-      <c r="J46">
-        <v>0</v>
+      <c r="J46" s="3">
+        <v>22</v>
       </c>
       <c r="K46" s="1">
         <v>1</v>
@@ -8808,7 +8827,7 @@
       <c r="BB46" s="1">
         <v>1</v>
       </c>
-      <c r="BC46">
+      <c r="BC46" s="5">
         <v>0</v>
       </c>
       <c r="BD46">

</xml_diff>

<commit_message>
Level 4 added ----- Level 4 enemies and objective added
</commit_message>
<xml_diff>
--- a/Base/TileMap/Formatting/Level4.xlsx
+++ b/Base/TileMap/Formatting/Level4.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Level4" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -864,10 +863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BI56"/>
+  <dimension ref="A1:BE56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BJ23" sqref="BJ23"/>
+      <selection activeCell="BI22" sqref="BI22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3176,16 +3175,16 @@
       <c r="Q14" s="5">
         <v>0</v>
       </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
+      <c r="R14" s="5">
+        <v>0</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0</v>
+      </c>
+      <c r="T14" s="5">
+        <v>0</v>
+      </c>
+      <c r="U14" s="5">
         <v>0</v>
       </c>
       <c r="V14" s="5">
@@ -3230,16 +3229,16 @@
       <c r="AI14" s="5">
         <v>0</v>
       </c>
-      <c r="AJ14">
-        <v>0</v>
-      </c>
-      <c r="AK14">
-        <v>0</v>
-      </c>
-      <c r="AL14">
-        <v>0</v>
-      </c>
-      <c r="AM14">
+      <c r="AJ14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM14" s="5">
         <v>0</v>
       </c>
       <c r="AN14" s="5">
@@ -3643,7 +3642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -3816,7 +3815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -3989,7 +3988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -4162,7 +4161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -4335,7 +4334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -4508,7 +4507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1</v>
       </c>
@@ -4680,12 +4679,8 @@
       <c r="BE22" s="1">
         <v>1</v>
       </c>
-      <c r="BI22">
-        <f>51-4</f>
-        <v>47</v>
-      </c>
     </row>
-    <row r="23" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -4858,7 +4853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -5031,7 +5026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -5204,7 +5199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>1</v>
       </c>
@@ -5377,7 +5372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -5483,16 +5478,16 @@
       <c r="AI27" s="5">
         <v>0</v>
       </c>
-      <c r="AJ27">
-        <v>0</v>
-      </c>
-      <c r="AK27">
-        <v>0</v>
-      </c>
-      <c r="AL27">
-        <v>0</v>
-      </c>
-      <c r="AM27">
+      <c r="AJ27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM27" s="5">
         <v>0</v>
       </c>
       <c r="AN27" s="5">
@@ -5550,7 +5545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -5723,7 +5718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -5896,7 +5891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -6069,7 +6064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>1</v>
       </c>
@@ -6242,7 +6237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -7508,16 +7503,16 @@
       <c r="R39" s="5">
         <v>0</v>
       </c>
-      <c r="S39">
-        <v>0</v>
-      </c>
-      <c r="T39">
-        <v>0</v>
-      </c>
-      <c r="U39">
-        <v>0</v>
-      </c>
-      <c r="V39">
+      <c r="S39" s="5">
+        <v>0</v>
+      </c>
+      <c r="T39" s="5">
+        <v>0</v>
+      </c>
+      <c r="U39" s="5">
+        <v>0</v>
+      </c>
+      <c r="V39" s="5">
         <v>0</v>
       </c>
       <c r="W39" s="5">
@@ -7559,16 +7554,16 @@
       <c r="AI39" s="5">
         <v>0</v>
       </c>
-      <c r="AJ39">
-        <v>0</v>
-      </c>
-      <c r="AK39">
-        <v>0</v>
-      </c>
-      <c r="AL39">
-        <v>0</v>
-      </c>
-      <c r="AM39">
+      <c r="AJ39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL39" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM39" s="5">
         <v>0</v>
       </c>
       <c r="AN39" s="5">

</xml_diff>